<commit_message>
[skrypt do updatowania wiki]-dodanie źródła w każdej linii
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,8 +437,16 @@
           <t>Q406</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr"/>
       <c r="G1" t="inlineStr"/>
       <c r="H1" t="inlineStr"/>
@@ -449,6 +457,8 @@
       <c r="M1" t="inlineStr"/>
       <c r="N1" t="inlineStr"/>
       <c r="O1" t="inlineStr"/>
+      <c r="P1" t="inlineStr"/>
+      <c r="Q1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,8 +476,16 @@
           <t>Q403</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -478,6 +496,8 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -495,8 +515,16 @@
           <t>"Papież Bonifacy IX przyznaje Małgorzacie, wdowie po mieszczaninie wrocławskim Johannesie von Sitten, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -507,6 +535,8 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -554,12 +584,22 @@
           <t>"185v"</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -577,8 +617,16 @@
           <t>+1394-04-23T00:00:00Z/11</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -589,6 +637,8 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -606,8 +656,16 @@
           <t>Q31</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -618,6 +676,8 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -645,8 +705,16 @@
           <t>Q386</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -655,6 +723,8 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -684,6 +754,8 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -713,6 +785,8 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -758,6 +832,8 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -787,6 +863,8 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -816,6 +894,8 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -845,6 +925,8 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -874,6 +956,8 @@
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -891,8 +975,16 @@
           <t>Q402</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -903,6 +995,8 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -920,8 +1014,16 @@
           <t>Q406</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
@@ -932,6 +1034,8 @@
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -949,8 +1053,16 @@
           <t>Q403</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
@@ -961,6 +1073,8 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -978,8 +1092,16 @@
           <t>"Papież Bonifacy IX przyznaje Pawłowi s. Nankera z Wierzchoniowa, kanonikowi krakowskiemu, łaskę, by w obliczu śmierci wybrany przez Pawła spowiednik mógł jeden raz udzielić mu mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
@@ -990,6 +1112,8 @@
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1037,12 +1161,22 @@
           <t>"172v"</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1060,8 +1194,16 @@
           <t>+1394-01-06T00:00:00Z/11</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -1072,6 +1214,8 @@
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1089,8 +1233,16 @@
           <t>Q31</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
@@ -1101,6 +1253,8 @@
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1128,8 +1282,16 @@
           <t>Q386</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -1138,6 +1300,8 @@
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1167,6 +1331,8 @@
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1196,6 +1362,8 @@
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1241,6 +1409,8 @@
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1270,6 +1440,8 @@
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1299,6 +1471,8 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1328,6 +1502,8 @@
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1357,6 +1533,8 @@
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1374,8 +1552,16 @@
           <t>Q402</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
@@ -1386,6 +1572,8 @@
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1403,8 +1591,16 @@
           <t>Q406</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
@@ -1415,6 +1611,8 @@
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1432,8 +1630,16 @@
           <t>Q403</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
@@ -1444,6 +1650,8 @@
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1461,8 +1669,16 @@
           <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
@@ -1473,6 +1689,8 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1520,12 +1738,22 @@
           <t>"172v"</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1543,8 +1771,16 @@
           <t>+1394-01-04T00:00:00Z/11</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
@@ -1555,6 +1791,8 @@
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1572,8 +1810,16 @@
           <t>Q31</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
@@ -1584,6 +1830,8 @@
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1611,8 +1859,16 @@
           <t>Q386</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
@@ -1621,6 +1877,8 @@
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1650,6 +1908,8 @@
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1679,6 +1939,8 @@
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1708,6 +1970,8 @@
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1737,6 +2001,8 @@
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1782,6 +2048,8 @@
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1811,6 +2079,8 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1840,6 +2110,8 @@
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1869,6 +2141,8 @@
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1898,6 +2172,8 @@
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1927,6 +2203,8 @@
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1944,8 +2222,16 @@
           <t>Q402</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
@@ -1956,6 +2242,8 @@
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1973,8 +2261,16 @@
           <t>Q406</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
@@ -1985,6 +2281,8 @@
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2002,8 +2300,16 @@
           <t>Q403</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
@@ -2014,6 +2320,8 @@
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2031,8 +2339,16 @@
           <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
@@ -2043,6 +2359,8 @@
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2090,12 +2408,22 @@
           <t>"172v"</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2113,8 +2441,16 @@
           <t>+1393-12-09T00:00:00Z/11</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
@@ -2125,6 +2461,8 @@
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2142,8 +2480,16 @@
           <t>Q31</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
@@ -2154,6 +2500,8 @@
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2181,8 +2529,16 @@
           <t>Q385</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
@@ -2191,6 +2547,8 @@
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2220,6 +2578,8 @@
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2249,6 +2609,8 @@
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2294,6 +2656,8 @@
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2323,6 +2687,8 @@
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2352,6 +2718,8 @@
       <c r="M60" t="inlineStr"/>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2381,6 +2749,8 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2410,6 +2780,8 @@
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2439,6 +2811,8 @@
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2456,8 +2830,16 @@
           <t>Q402</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
@@ -2468,6 +2850,8 @@
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2485,8 +2869,16 @@
           <t>Q392</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
@@ -2497,6 +2889,8 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2514,8 +2908,16 @@
           <t>Q387</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
@@ -2526,6 +2928,8 @@
       <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2543,8 +2947,16 @@
           <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
@@ -2555,6 +2967,8 @@
       <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2612,10 +3026,20 @@
           <t>"CCLVII-CCLVIII"</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr"/>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2633,8 +3057,16 @@
           <t>+1389-11-13T00:00:00Z/11</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
@@ -2645,6 +3077,8 @@
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2662,8 +3096,16 @@
           <t>Q31</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
@@ -2674,6 +3116,8 @@
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2701,8 +3145,16 @@
           <t>Q385</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
@@ -2711,6 +3163,8 @@
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2738,8 +3192,16 @@
           <t>Q386</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
@@ -2748,6 +3210,8 @@
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2775,8 +3239,16 @@
           <t>Q386</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
@@ -2785,6 +3257,8 @@
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2814,6 +3288,8 @@
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2843,6 +3319,8 @@
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2872,6 +3350,8 @@
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2901,6 +3381,8 @@
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2930,6 +3412,8 @@
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2975,6 +3459,8 @@
       <c r="M79" t="inlineStr"/>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3004,6 +3490,8 @@
       <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3033,6 +3521,8 @@
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3062,6 +3552,8 @@
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3091,6 +3583,8 @@
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3120,6 +3614,8 @@
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3149,6 +3645,8 @@
       <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3178,6 +3676,8 @@
       <c r="M86" t="inlineStr"/>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3207,6 +3707,8 @@
       <c r="M87" t="inlineStr"/>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3236,6 +3738,8 @@
       <c r="M88" t="inlineStr"/>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3265,6 +3769,8 @@
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3294,6 +3800,8 @@
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3311,8 +3819,16 @@
           <t>Q402</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
@@ -3323,6 +3839,8 @@
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3340,8 +3858,16 @@
           <t>Q392</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr"/>
@@ -3352,6 +3878,8 @@
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3369,8 +3897,16 @@
           <t>Q434</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
@@ -3381,6 +3917,8 @@
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3398,8 +3936,16 @@
           <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
@@ -3410,6 +3956,8 @@
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3468,10 +4016,20 @@
           <t>"CCLVIII-CCLVIIII"</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3489,8 +4047,16 @@
           <t>+1389-11-13T00:00:00Z/11</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
@@ -3501,6 +4067,8 @@
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3518,8 +4086,16 @@
           <t>Q31</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
@@ -3530,6 +4106,8 @@
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3557,8 +4135,16 @@
           <t>Q385</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
@@ -3567,6 +4153,8 @@
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3594,8 +4182,16 @@
           <t>Q386</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr"/>
@@ -3604,6 +4200,8 @@
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3633,6 +4231,8 @@
       <c r="M100" t="inlineStr"/>
       <c r="N100" t="inlineStr"/>
       <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3662,6 +4262,8 @@
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="inlineStr"/>
       <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3691,6 +4293,8 @@
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr"/>
       <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3720,6 +4324,8 @@
       <c r="M103" t="inlineStr"/>
       <c r="N103" t="inlineStr"/>
       <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3749,6 +4355,8 @@
       <c r="M104" t="inlineStr"/>
       <c r="N104" t="inlineStr"/>
       <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3778,6 +4386,8 @@
       <c r="M105" t="inlineStr"/>
       <c r="N105" t="inlineStr"/>
       <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3823,6 +4433,8 @@
       <c r="M106" t="inlineStr"/>
       <c r="N106" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3860,6 +4472,8 @@
       <c r="M107" t="inlineStr"/>
       <c r="N107" t="inlineStr"/>
       <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3889,6 +4503,8 @@
       <c r="M108" t="inlineStr"/>
       <c r="N108" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3918,6 +4534,8 @@
       <c r="M109" t="inlineStr"/>
       <c r="N109" t="inlineStr"/>
       <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3947,6 +4565,8 @@
       <c r="M110" t="inlineStr"/>
       <c r="N110" t="inlineStr"/>
       <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3976,6 +4596,8 @@
       <c r="M111" t="inlineStr"/>
       <c r="N111" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4005,6 +4627,8 @@
       <c r="M112" t="inlineStr"/>
       <c r="N112" t="inlineStr"/>
       <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4034,6 +4658,8 @@
       <c r="M113" t="inlineStr"/>
       <c r="N113" t="inlineStr"/>
       <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4063,6 +4689,8 @@
       <c r="M114" t="inlineStr"/>
       <c r="N114" t="inlineStr"/>
       <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4092,6 +4720,8 @@
       <c r="M115" t="inlineStr"/>
       <c r="N115" t="inlineStr"/>
       <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[skrypt do updatowania wiki]-najnowsze wyniki
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -742,8 +742,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -773,8 +781,16 @@
           <t>"Margarete, relicte quondam Iohannis de Sitten civis Wratislauiensis"</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -824,8 +840,16 @@
           <t>14</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -851,8 +875,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -882,8 +914,16 @@
           <t>Q442</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
@@ -913,8 +953,16 @@
           <t>Q443</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -944,8 +992,16 @@
           <t>Q30</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Q476</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
@@ -1319,8 +1375,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
@@ -1350,8 +1414,16 @@
           <t>Q441</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
@@ -1401,8 +1473,16 @@
           <t>14</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -1428,8 +1508,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
@@ -1459,8 +1547,16 @@
           <t>Q441</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
@@ -1490,8 +1586,16 @@
           <t>Q30</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
@@ -1521,8 +1625,16 @@
           <t>Q149</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Q475</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
@@ -1896,8 +2008,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
@@ -1927,8 +2047,16 @@
           <t>Q436</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
@@ -1958,8 +2086,16 @@
           <t>Q436</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
@@ -1989,8 +2125,16 @@
           <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
@@ -2040,8 +2184,16 @@
           <t>14</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2067,8 +2219,16 @@
           <t>Q372</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
@@ -2098,8 +2258,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
@@ -2129,8 +2297,16 @@
           <t>Q436</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
@@ -2160,8 +2336,16 @@
           <t>Q437</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
@@ -2191,8 +2375,16 @@
           <t>Q30</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
@@ -2566,8 +2758,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
@@ -2597,8 +2797,16 @@
           <t>Q404</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
@@ -2648,8 +2856,16 @@
           <t>14</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
@@ -2675,8 +2891,16 @@
           <t>Q372</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
@@ -2706,8 +2930,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
@@ -2737,8 +2969,16 @@
           <t>Q404</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
@@ -2768,8 +3008,16 @@
           <t>Q413</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
@@ -2799,8 +3047,16 @@
           <t>Q30</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
@@ -3276,8 +3532,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
@@ -3307,8 +3571,16 @@
           <t>Q391</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
@@ -3338,8 +3610,16 @@
           <t>Q393</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
@@ -3369,8 +3649,16 @@
           <t>Q394</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
@@ -3400,8 +3688,16 @@
           <t>"C(ancellaria)"</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
@@ -3451,8 +3747,16 @@
           <t>24</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
@@ -3478,8 +3782,16 @@
           <t>Q139</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
@@ -3509,8 +3821,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
@@ -3540,8 +3860,16 @@
           <t>Q393</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
@@ -3571,8 +3899,16 @@
           <t>Q30</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
@@ -3602,8 +3938,16 @@
           <t>Q391</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
@@ -3633,8 +3977,16 @@
           <t>Q142</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
@@ -3664,8 +4016,16 @@
           <t>Q394</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
@@ -3695,8 +4055,16 @@
           <t>Q118</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
@@ -3726,8 +4094,16 @@
           <t>Q398</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
@@ -3757,8 +4133,16 @@
           <t>Q149</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
@@ -3788,8 +4172,16 @@
           <t>Q146</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
@@ -4219,8 +4611,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
@@ -4250,8 +4650,16 @@
           <t>Q430</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
@@ -4281,8 +4689,16 @@
           <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
@@ -4312,8 +4728,16 @@
           <t>Q426</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
@@ -4343,8 +4767,16 @@
           <t>Q424</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
@@ -4374,8 +4806,16 @@
           <t>"C(ancellaria)"</t>
         </is>
       </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
@@ -4425,8 +4865,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr"/>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
@@ -4491,8 +4939,16 @@
           <t>Q10</t>
         </is>
       </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="inlineStr"/>
@@ -4522,8 +4978,16 @@
           <t>Q423</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr"/>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
@@ -4553,8 +5017,16 @@
           <t>Q30</t>
         </is>
       </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr"/>
@@ -4584,8 +5056,16 @@
           <t>Q432</t>
         </is>
       </c>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr"/>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="inlineStr"/>
@@ -4615,8 +5095,16 @@
           <t>Q429</t>
         </is>
       </c>
-      <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
@@ -4646,8 +5134,16 @@
           <t>Q430</t>
         </is>
       </c>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="inlineStr"/>
@@ -4677,8 +5173,16 @@
           <t>Q469</t>
         </is>
       </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr"/>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
@@ -4708,8 +5212,16 @@
           <t>Q427</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr"/>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>

</xml_diff>

<commit_message>
[skrypt do updatowania wiki]-wyniki na nowozaładowanych tekstach po poprawkach
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q115"/>
+  <dimension ref="A1:Q123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -862,31 +862,39 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Q442</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>P56</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Q443</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Q476</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>P27</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Q10</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Q476</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -901,31 +909,39 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Q443</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>P33</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Q442</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Q476</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>P27</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Q442</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Q476</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -950,7 +966,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Q443</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -989,7 +1005,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q442</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1018,17 +1034,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q443</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1038,7 +1054,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -1057,17 +1073,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1077,7 +1093,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -1101,12 +1117,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1140,12 +1156,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Pawłowi s. Nankera z Wierzchoniowa, kanonikowi krakowskiemu, łaskę, by w obliczu śmierci wybrany przez Pawła spowiednik mógł jeden raz udzielić mu mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1179,54 +1195,30 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
           <t>Q475</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
@@ -1242,12 +1234,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>+1394-01-06T00:00:00Z/11</t>
+          <t>"Papież Bonifacy IX przyznaje Pawłowi s. Nankera z Wierzchoniowa, kanonikowi krakowskiemu, łaskę, by w obliczu śmierci wybrany przez Pawła spowiednik mógł jeden raz udzielić mu mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1281,30 +1273,54 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
           <t>Q475</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
@@ -1320,34 +1336,26 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"BP 3, nr 354"</t>
+          <t>+1394-01-06T00:00:00Z/11</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
           <t>Q475</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -1367,12 +1375,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1406,26 +1414,34 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Q441</t>
+          <t>"BP 3, nr 354"</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Q475</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -1445,44 +1461,28 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to"</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
           <t>Q475</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -1500,12 +1500,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1539,28 +1539,44 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Q441</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to"</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>Q475</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -1583,7 +1599,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1622,7 +1638,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1651,17 +1667,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1671,7 +1687,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -1690,17 +1706,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1710,7 +1726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -1729,17 +1745,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1749,7 +1765,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
@@ -1768,17 +1784,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q392</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1788,7 +1804,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1807,59 +1823,35 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q434</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
@@ -1870,17 +1862,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>+1394-01-04T00:00:00Z/11</t>
+          <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1890,7 +1882,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1909,37 +1901,70 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>"ASV, Reg. Lat., vol. 6, f. 258v-259v (or. f.
+                     CCLVIII-CCLVIIII)"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Q474</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Q382</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>"258v-259v"</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>"CCLVIII-CCLVIIII"</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
@@ -1948,39 +1973,31 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>"BP 3, nr 353"</t>
+          <t>+1389-11-13T00:00:00Z/11</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
@@ -1995,17 +2012,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2015,7 +2032,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -2034,31 +2051,39 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>"MPV 8, nr 39"</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Q474</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -2073,31 +2098,39 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>"RG 2, nr 05764"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Q474</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
@@ -2112,17 +2145,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P38</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2132,7 +2165,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
@@ -2151,49 +2184,33 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2206,17 +2223,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Q372</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2226,7 +2243,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F43" t="inlineStr"/>
@@ -2245,17 +2262,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P52</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2265,7 +2282,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F44" t="inlineStr"/>
@@ -2284,17 +2301,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2304,7 +2321,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F45" t="inlineStr"/>
@@ -2323,17 +2340,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P42</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Q437</t>
+          <t>Q426</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2343,7 +2360,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
@@ -2362,17 +2379,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P42</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q424</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2382,7 +2399,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
@@ -2401,17 +2418,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>"C(ancellaria)"</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2421,7 +2438,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
@@ -2440,33 +2457,49 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>"N(icolaus). XXI. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Q400</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Q470</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2479,17 +2512,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P29</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q416</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2499,7 +2532,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -2518,17 +2551,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2538,7 +2571,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
@@ -2557,59 +2590,35 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr"/>
@@ -2620,17 +2629,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>+1393-12-09T00:00:00Z/11</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2640,7 +2649,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F53" t="inlineStr"/>
@@ -2659,17 +2668,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2679,7 +2688,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
@@ -2698,39 +2707,31 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>"BP 3, nr 349 (false sub data 9 XI 1393)"</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
@@ -2745,17 +2746,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2765,7 +2766,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
@@ -2784,17 +2785,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q469</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2804,7 +2805,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
@@ -2823,49 +2824,33 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
@@ -2878,17 +2863,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Q372</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2898,7 +2883,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -2917,17 +2902,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2937,7 +2922,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -2956,17 +2941,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2976,7 +2961,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2995,17 +2980,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3015,7 +3000,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -3034,35 +3019,59 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Q400</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr"/>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
@@ -3073,17 +3082,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>+1394-01-04T00:00:00Z/11</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3093,7 +3102,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -3112,17 +3121,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Q392</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -3132,7 +3141,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
@@ -3151,31 +3160,39 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Q387</t>
+          <t>"BP 3, nr 353"</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
@@ -3190,17 +3207,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3210,7 +3227,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
@@ -3229,69 +3246,37 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 6, f. 257r-258v (or. f. CCLVII-CCLVIII)"</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Q382</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>"257r-258v"</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>"CCLVII-CCLVIII"</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q474</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
@@ -3300,17 +3285,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>+1389-11-13T00:00:00Z/11</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3320,7 +3305,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
@@ -3339,17 +3324,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3359,7 +3344,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
@@ -3378,41 +3363,49 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"MPV 8, nr 31"</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Q385</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P30</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
@@ -3425,27 +3418,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"BP 3, nr 111"</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Q386</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3455,7 +3448,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
@@ -3472,27 +3465,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>"RG 2, nr 05985"</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Q386</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3502,7 +3495,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -3519,17 +3512,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q372</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3539,7 +3532,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
@@ -3558,17 +3551,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Q391</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3578,7 +3571,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
@@ -3597,17 +3590,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3617,7 +3610,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
@@ -3636,17 +3629,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>P52</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3656,7 +3649,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
@@ -3675,17 +3668,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>"C(ancellaria)"</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3695,7 +3688,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
@@ -3714,49 +3707,33 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>"N(icolaus). XXIIII. de Ben(even)to."</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
@@ -3769,17 +3746,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Q139</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3789,7 +3766,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -3808,17 +3785,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3828,7 +3805,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
@@ -3847,17 +3824,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3867,7 +3844,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
@@ -3886,35 +3863,59 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr"/>
-      <c r="K83" t="inlineStr"/>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="L83" t="inlineStr"/>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
@@ -3925,17 +3926,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Q391</t>
+          <t>+1393-12-09T00:00:00Z/11</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3945,7 +3946,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
@@ -3964,17 +3965,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Q142</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3984,7 +3985,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -4003,31 +4004,39 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>"BP 3, nr 349 (false sub data 9 XI 1393)"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
@@ -4042,17 +4051,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Q118</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -4062,7 +4071,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -4081,17 +4090,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Q398</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -4101,7 +4110,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
@@ -4120,33 +4129,49 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
-      <c r="I89" t="inlineStr"/>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
@@ -4159,17 +4184,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Q146</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4179,11 +4204,19 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr"/>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
@@ -4198,17 +4231,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -4218,11 +4251,19 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Q470</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
@@ -4237,17 +4278,17 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Q392</t>
+          <t>Q372</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -4257,7 +4298,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
@@ -4276,17 +4317,17 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Q434</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -4296,7 +4337,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
@@ -4315,17 +4356,17 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -4335,7 +4376,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
@@ -4354,70 +4395,37 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>"ASV, Reg. Lat., vol. 6, f. 258v-259v (or. f.
-                     CCLVIII-CCLVIIII)"</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Q382</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>"258v-259v"</t>
-        </is>
-      </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>"CCLVIII-CCLVIIII"</t>
-        </is>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>Q470</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr"/>
@@ -4426,17 +4434,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>+1389-11-13T00:00:00Z/11</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -4446,7 +4454,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F96" t="inlineStr"/>
@@ -4465,17 +4473,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -4485,7 +4493,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -4504,39 +4512,31 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>"MPV 8, nr 39"</t>
+          <t>Q392</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>Q470</t>
-        </is>
-      </c>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
@@ -4551,39 +4551,31 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>"RG 2, nr 05764"</t>
+          <t>Q387</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>Q470</t>
-        </is>
-      </c>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr"/>
@@ -4598,17 +4590,17 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4618,7 +4610,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
@@ -4637,37 +4629,69 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>P52</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>"AAV, Reg. Lat., vol. 6, f. 257r-258v (or. f. CCLVII-CCLVIII)"</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Q470</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Q382</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>"257r-258v"</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>"CCLVII-CCLVIII"</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="N101" t="inlineStr"/>
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr"/>
@@ -4676,17 +4700,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>P38</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
+          <t>+1389-11-13T00:00:00Z/11</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4696,7 +4720,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
@@ -4715,17 +4739,17 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>P42</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Q426</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -4735,7 +4759,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
@@ -4754,31 +4778,39 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>P42</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Q424</t>
+          <t>"MPV 8, nr 31"</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Q470</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr"/>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
@@ -4793,31 +4825,39 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>"C(ancellaria)"</t>
+          <t>"BP 3, nr 111"</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Q470</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
@@ -4832,49 +4872,41 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>"N(icolaus). XXI. de Ben(even)to."</t>
+          <t>"RG 2, nr 05985"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q386</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>P30</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>Q470</t>
-        </is>
-      </c>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
@@ -4887,17 +4919,17 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>P29</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Q416</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4907,7 +4939,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F107" t="inlineStr"/>
@@ -4926,17 +4958,17 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q391</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4946,7 +4978,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F108" t="inlineStr"/>
@@ -4965,17 +4997,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4985,7 +5017,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F109" t="inlineStr"/>
@@ -5004,17 +5036,17 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P52</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q394</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -5024,7 +5056,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F110" t="inlineStr"/>
@@ -5043,17 +5075,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>"C(ancellaria)"</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -5063,7 +5095,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F111" t="inlineStr"/>
@@ -5082,33 +5114,49 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>"N(icolaus). XXIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Q470</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr"/>
-      <c r="G112" t="inlineStr"/>
-      <c r="H112" t="inlineStr"/>
-      <c r="I112" t="inlineStr"/>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
@@ -5121,17 +5169,17 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q394</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>Q139</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -5141,7 +5189,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F113" t="inlineStr"/>
@@ -5160,7 +5208,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -5170,7 +5218,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Q469</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -5180,7 +5228,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
@@ -5199,7 +5247,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -5209,7 +5257,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Q427</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -5219,7 +5267,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="F115" t="inlineStr"/>
@@ -5235,6 +5283,318 @@
       <c r="P115" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
     </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+      <c r="Q116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Q391</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Q142</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+      <c r="K118" t="inlineStr"/>
+      <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
+      <c r="P118" t="inlineStr"/>
+      <c r="Q118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Q394</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr"/>
+      <c r="P119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Q118</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Q398</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
+      <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" t="inlineStr"/>
+      <c r="Q121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Q149</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+      <c r="K122" t="inlineStr"/>
+      <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Q146</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+      <c r="K123" t="inlineStr"/>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[skrypt do updatowania wiki]-poprawione błędy (status beneficjów + podwójne źródło dla mąż/żona/ojciec/syn
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q123"/>
+  <dimension ref="A1:Q135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>+1394-04-23T00:00:00Z/11</t>
+          <t>+1394-04-23T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>+1394-01-06T00:00:00Z/11</t>
+          <t>+1394-01-06T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1589,17 +1589,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1628,12 +1628,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1745,17 +1745,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
@@ -1784,17 +1784,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Q392</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
@@ -1828,12 +1828,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Q434</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1867,12 +1867,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
+          <t>Q392</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1906,65 +1906,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>"ASV, Reg. Lat., vol. 6, f. 258v-259v (or. f.
-                     CCLVIII-CCLVIIII)"</t>
+          <t>Q434</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Q382</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>"258v-259v"</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>"CCLVIII-CCLVIIII"</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
           <t>Q470</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
@@ -1978,12 +1945,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>+1389-11-13T00:00:00Z/11</t>
+          <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2017,32 +1984,65 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>"ASV, Reg. Lat., vol. 6, f. 258v-259v (or. f.
+                     CCLVIII-CCLVIIII)"</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Q382</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>"258v-259v"</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>"CCLVIII-CCLVIIII"</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
@@ -2056,34 +2056,26 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>"MPV 8, nr 39"</t>
+          <t>+1389-11-13T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
           <t>Q470</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -2103,34 +2095,26 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>"RG 2, nr 05764"</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
           <t>Q470</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
@@ -2150,26 +2134,34 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"MPV 8, nr 39"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
@@ -2189,26 +2181,34 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>"RG 2, nr 05764"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
@@ -2228,12 +2228,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2267,12 +2267,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P52</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2301,17 +2301,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>P25</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>Q423</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>P38</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2340,17 +2340,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P42</t>
+          <t>P52</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Q426</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2384,12 +2384,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P42</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Q424</t>
+          <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2418,17 +2418,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P42</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"C(ancellaria)"</t>
+          <t>Q426</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2457,49 +2457,33 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Q423</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>P42</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Q424</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>P34</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>"N(icolaus). XXI. de Ben(even)to."</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>P31</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>Q470</t>
-        </is>
-      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2512,17 +2496,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P29</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Q416</t>
+          <t>"C(ancellaria)"</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2556,28 +2540,44 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"N(icolaus). XXI. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -2590,17 +2590,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2629,17 +2629,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2668,17 +2668,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2707,17 +2707,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2746,17 +2746,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2785,17 +2785,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Q469</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2824,17 +2824,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P54</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Q427</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2863,17 +2863,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P28</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -2902,17 +2902,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P29</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>Q416</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -2941,17 +2941,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2980,17 +2980,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -3019,59 +3019,35 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
@@ -3082,17 +3058,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>+1394-01-04T00:00:00Z/11</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3102,7 +3078,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
@@ -3121,17 +3097,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -3141,7 +3117,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
@@ -3160,39 +3136,31 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>"BP 3, nr 353"</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
@@ -3207,17 +3175,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q469</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3227,7 +3195,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
@@ -3246,17 +3214,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3266,7 +3234,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -3290,12 +3258,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3324,17 +3292,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P38</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3368,44 +3336,28 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
           <t>Q474</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
@@ -3418,17 +3370,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P56</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Q437</t>
+          <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3441,16 +3393,8 @@
           <t>Q474</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
@@ -3465,43 +3409,59 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Q437</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>P33</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
           <t>Q474</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
-      <c r="J73" t="inlineStr"/>
-      <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
@@ -3512,17 +3472,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Q372</t>
+          <t>+1394-01-04T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3556,12 +3516,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3595,26 +3555,34 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>"BP 3, nr 353"</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
           <t>Q474</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
@@ -3634,12 +3602,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Q437</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3673,12 +3641,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3707,17 +3675,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3727,7 +3695,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
@@ -3746,17 +3714,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3766,7 +3734,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
@@ -3785,33 +3753,49 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Q400</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr"/>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
@@ -3824,17 +3808,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3844,11 +3828,19 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Q400</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr"/>
+          <t>Q474</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Q474</t>
+        </is>
+      </c>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
@@ -3863,59 +3855,43 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Q388</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>P14</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+          <t>Q474</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
@@ -3926,17 +3902,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>+1393-12-09T00:00:00Z/11</t>
+          <t>Q372</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3946,7 +3922,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
@@ -3965,17 +3941,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3985,7 +3961,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
@@ -4004,39 +3980,31 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>"BP 3, nr 349 (false sub data 9 XI 1393)"</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+          <t>Q474</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
@@ -4051,17 +4019,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -4071,7 +4039,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -4090,17 +4058,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -4110,7 +4078,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
@@ -4134,44 +4102,28 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
           <t>Q400</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
@@ -4184,17 +4136,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>P56</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4207,16 +4159,8 @@
           <t>Q400</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
@@ -4231,17 +4175,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>P33</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -4254,16 +4198,8 @@
           <t>Q400</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
@@ -4278,17 +4214,17 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Q372</t>
+          <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -4322,30 +4258,54 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
           <t>Q400</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
@@ -4361,12 +4321,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>+1393-12-09T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -4400,12 +4360,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -4439,26 +4399,34 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>"BP 3, nr 349 (false sub data 9 XI 1393)"</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
           <t>Q400</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr"/>
@@ -4473,17 +4441,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -4493,7 +4461,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
@@ -4512,17 +4480,17 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Q392</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -4532,7 +4500,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
@@ -4551,33 +4519,49 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Q387</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
-      <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr"/>
@@ -4590,17 +4574,17 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4610,11 +4594,19 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Q381</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="inlineStr"/>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Q400</t>
+        </is>
+      </c>
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
@@ -4629,69 +4621,45 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 6, f. 257r-258v (or. f. CCLVII-CCLVIII)"</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Q388</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>P14</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Q382</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>"257r-258v"</t>
-        </is>
-      </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>"CCLVII-CCLVIII"</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
       <c r="N101" t="inlineStr"/>
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr"/>
@@ -4700,17 +4668,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>+1389-11-13T00:00:00Z/11</t>
+          <t>Q372</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4720,7 +4688,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
@@ -4739,17 +4707,17 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -4759,7 +4727,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
@@ -4778,39 +4746,31 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>"MPV 8, nr 31"</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
@@ -4825,39 +4785,31 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>"BP 3, nr 111"</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
@@ -4872,39 +4824,31 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>"RG 2, nr 05985"</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
@@ -4924,12 +4868,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4963,12 +4907,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Q391</t>
+          <t>Q392</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -5002,12 +4946,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>Q387</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -5041,12 +4985,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>P52</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -5080,32 +5024,64 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>"C(ancellaria)"</t>
+          <t>"AAV, Reg. Lat., vol. 6, f. 257r-258v (or. f. CCLVII-CCLVIII)"</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Q382</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>"257r-258v"</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>"CCLVII-CCLVIII"</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr"/>
-      <c r="J111" t="inlineStr"/>
-      <c r="K111" t="inlineStr"/>
-      <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr"/>
       <c r="N111" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
       <c r="P111" t="inlineStr"/>
@@ -5119,44 +5095,28 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>"N(icolaus). XXIIII. de Ben(even)to."</t>
+          <t>+1389-11-13T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr">
-        <is>
           <t>Q381</t>
         </is>
       </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
@@ -5169,17 +5129,17 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Q139</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -5213,26 +5173,34 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"MPV 8, nr 31"</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr"/>
-      <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
@@ -5252,26 +5220,34 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>"BP 3, nr 111"</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr"/>
-      <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
@@ -5291,26 +5267,34 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>"RG 2, nr 05985"</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr"/>
@@ -5330,12 +5314,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Q391</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -5369,12 +5353,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Q142</t>
+          <t>Q391</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -5408,12 +5392,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -5447,12 +5431,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P52</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Q118</t>
+          <t>Q394</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -5486,12 +5470,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Q398</t>
+          <t>"C(ancellaria)"</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -5525,28 +5509,44 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>"N(icolaus). XXIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr"/>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
-      <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
@@ -5559,17 +5559,17 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Q146</t>
+          <t>Q142</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -5595,6 +5595,474 @@
       <c r="P123" t="inlineStr"/>
       <c r="Q123" t="inlineStr"/>
     </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Q142</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>P35</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Q394</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Q139</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
+      <c r="K125" t="inlineStr"/>
+      <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" t="inlineStr"/>
+      <c r="O125" t="inlineStr"/>
+      <c r="P125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Q10</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
+      <c r="K127" t="inlineStr"/>
+      <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" t="inlineStr"/>
+      <c r="Q127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
+      <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr"/>
+      <c r="O128" t="inlineStr"/>
+      <c r="P128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Q391</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Q142</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
+      <c r="K130" t="inlineStr"/>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Q394</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
+      <c r="K131" t="inlineStr"/>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Q118</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
+      <c r="K132" t="inlineStr"/>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Q398</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
+      <c r="K133" t="inlineStr"/>
+      <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" t="inlineStr"/>
+      <c r="O133" t="inlineStr"/>
+      <c r="P133" t="inlineStr"/>
+      <c r="Q133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Q149</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr"/>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr"/>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
+      <c r="K134" t="inlineStr"/>
+      <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr"/>
+      <c r="O134" t="inlineStr"/>
+      <c r="P134" t="inlineStr"/>
+      <c r="Q134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Q146</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
+      <c r="L135" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
+      <c r="P135" t="inlineStr"/>
+      <c r="Q135" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[skrypt do updatowania wiki]-test3
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q135"/>
+  <dimension ref="A1:Q152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -768,17 +768,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Q476</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>P23</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Q442</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>P38</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>"Margarete, relicte quondam Iohannis de Sitten civis Wratislauiensis"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -812,44 +812,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q442</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
           <t>Q476</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -867,12 +851,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P56</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Q443</t>
+          <t>"Margarete, relicte quondam Iohannis de Sitten civis Wratislauiensis"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -885,16 +869,8 @@
           <t>Q476</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Q476</t>
-        </is>
-      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -909,41 +885,49 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Q443</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P33</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Q442</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>Q476</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Q476</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -956,17 +940,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Q476</t>
+          <t>Q442</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q443</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -995,12 +979,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Q476</t>
+          <t>Q443</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1044,7 +1028,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Q443</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1083,7 +1067,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q442</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1112,17 +1096,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q443</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1132,7 +1116,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -1151,17 +1135,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1171,7 +1155,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q476</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
@@ -1195,12 +1179,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1234,12 +1218,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Pawłowi s. Nankera z Wierzchoniowa, kanonikowi krakowskiemu, łaskę, by w obliczu śmierci wybrany przez Pawła spowiednik mógł jeden raz udzielić mu mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1273,54 +1257,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
           <t>Q475</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
@@ -1336,12 +1296,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>+1394-01-06T00:00:00Z/11/J</t>
+          <t>"Papież Bonifacy IX przyznaje Pawłowi s. Nankera z Wierzchoniowa, kanonikowi krakowskiemu, łaskę, by w obliczu śmierci wybrany przez Pawła spowiednik mógł jeden raz udzielić mu mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1375,30 +1335,54 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>Q475</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
@@ -1414,34 +1398,26 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>"BP 3, nr 354"</t>
+          <t>+1394-01-06T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
           <t>Q475</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
@@ -1461,12 +1437,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1500,26 +1476,34 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Q441</t>
+          <t>"BP 3, nr 354"</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Q475</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
@@ -1539,44 +1523,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to"</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
           <t>Q475</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -1589,17 +1557,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Q475</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>P23</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>Q441</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>P53</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Q149</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1628,12 +1596,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P35</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1667,17 +1635,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"Paulo Nankeri, canonico Cracouiensi"</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1711,28 +1679,44 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Q441</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
           <t>Q475</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -1745,17 +1729,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1784,17 +1768,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q475</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1823,17 +1807,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1843,7 +1827,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
@@ -1862,17 +1846,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Q392</t>
+          <t>Q441</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1882,7 +1866,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1901,17 +1885,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Q434</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1921,7 +1905,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
@@ -1940,17 +1924,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
+          <t>Q149</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1960,7 +1944,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q475</t>
         </is>
       </c>
       <c r="F37" t="inlineStr"/>
@@ -1984,65 +1968,32 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>"ASV, Reg. Lat., vol. 6, f. 258v-259v (or. f.
-                     CCLVIII-CCLVIIII)"</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Q382</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>"258v-259v"</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>"CCLVIII-CCLVIIII"</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
           <t>Q470</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
@@ -2056,12 +2007,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>+1389-11-13T00:00:00Z/11/J</t>
+          <t>Q392</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2095,12 +2046,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q434</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2134,34 +2085,26 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"MPV 8, nr 39"</t>
+          <t>"Papież Bonifacy IX poleca oficjałowi naumburskiemu, by mocą władzy apostolskiej udzielił Mikołajowi Kalow, mistrzowi sztuk i bakałarzowi medycyny, ekspektatywy na kanonię większą w kapitule miśnieńskiej, pomimo że Mikołaj posiada już kanonię lubuską oraz kanonię w kolegiacie NMP w Wurzen."</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
           <t>Q470</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
@@ -2181,40 +2124,64 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"RG 2, nr 05764"</t>
+          <t>"ASV, Reg. Lat., vol. 6, f. 258v-259v (or. f. CCLVIII-CCLVIIII)"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Q386</t>
+          <t>Q388</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P14</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
+          <t>Q382</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>"258v-259v"</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>"CCLVIII-CCLVIIII"</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
@@ -2228,12 +2195,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>+1389-11-13T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2267,12 +2234,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2306,26 +2273,34 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>"MPV 8, nr 39"</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -2345,26 +2320,34 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P52</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>"RG 2, nr 05764"</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
@@ -2379,17 +2362,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P38</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2418,17 +2401,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P42</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Q426</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2457,17 +2440,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Q470</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>P25</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>Q423</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>P42</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Q424</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2501,12 +2484,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P52</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>"C(ancellaria)"</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2535,49 +2518,33 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>Q423</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>P38</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>"Nicolaum Kalow, canonicum Lubucensem, qui, ut asserit, magister in artibus et bacallarius in medicina existit"</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>P34</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>"N(icolaus). XXI. de Ben(even)to."</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>P31</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>Q470</t>
-        </is>
-      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -2595,12 +2562,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P53</t>
+          <t>P42</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>Q426</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2629,17 +2596,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P35</t>
+          <t>P42</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q424</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2668,17 +2635,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P53</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>"C(ancellaria)"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2707,33 +2674,49 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P35</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>"N(icolaus). XXI. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
           <t>Q470</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
@@ -2756,7 +2739,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Q427</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2785,7 +2768,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Q427</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2829,12 +2812,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P54</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2863,12 +2846,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P28</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2902,17 +2885,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P29</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Q416</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2941,17 +2924,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2980,17 +2963,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P54</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Q423</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3019,17 +3002,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P28</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -3058,17 +3041,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Q470</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P29</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Q432</t>
+          <t>Q416</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3107,7 +3090,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Q429</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -3146,7 +3129,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Q430</t>
+          <t>Q423</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -3185,7 +3168,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Q469</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3224,7 +3207,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Q427</t>
+          <t>Q432</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3253,17 +3236,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q429</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3273,7 +3256,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
@@ -3292,17 +3275,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>Q430</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3312,7 +3295,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
@@ -3331,17 +3314,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q469</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3351,7 +3334,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
@@ -3370,17 +3353,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q427</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3390,7 +3373,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q470</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
@@ -3414,54 +3397,30 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
           <t>Q474</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
@@ -3477,12 +3436,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>+1394-01-04T00:00:00Z/11/J</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3516,12 +3475,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3555,34 +3514,26 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>"BP 3, nr 353"</t>
+          <t>"Papież Bonifacy IX przyznaje Lutce, żonie Krystyna z Zagórzyc, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
           <t>Q474</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
@@ -3602,30 +3553,54 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
           <t>Q474</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
-      <c r="J77" t="inlineStr"/>
-      <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
@@ -3641,12 +3616,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>+1394-01-04T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3680,12 +3655,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3714,31 +3689,39 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>P38</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
+          <t>"BP 3, nr 353"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
           <t>Q474</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
@@ -3758,44 +3741,28 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
           <t>Q474</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
@@ -3808,19 +3775,19 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>Q474</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>P23</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
           <t>Q436</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>P56</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Q437</t>
-        </is>
-      </c>
       <c r="D82" t="inlineStr">
         <is>
           <t>S51</t>
@@ -3831,16 +3798,8 @@
           <t>Q474</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
@@ -3855,12 +3814,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Q437</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>P33</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3878,16 +3837,8 @@
           <t>Q474</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Q474</t>
-        </is>
-      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr"/>
@@ -3907,12 +3858,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Q372</t>
+          <t>"Luthke, dilecti filii Cristini de Zageizicze uxori, Cracouiensis diocesis"</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3946,28 +3897,44 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
           <t>Q474</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
@@ -3980,17 +3947,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Q436</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -4019,17 +3986,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Q437</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -4058,17 +4025,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Q474</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q372</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -4097,17 +4064,17 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -4117,7 +4084,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
@@ -4136,17 +4103,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Q406</t>
+          <t>Q436</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4156,7 +4123,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
@@ -4175,17 +4142,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Q403</t>
+          <t>Q437</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -4195,7 +4162,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
@@ -4214,17 +4181,17 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -4234,7 +4201,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q474</t>
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
@@ -4258,54 +4225,30 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Q401</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>"172v"</t>
-        </is>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
           <t>Q400</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
@@ -4321,12 +4264,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>+1393-12-09T00:00:00Z/11/J</t>
+          <t>Q406</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -4360,12 +4303,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q403</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -4399,34 +4342,26 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>"BP 3, nr 349 (false sub data 9 XI 1393)"</t>
+          <t>"Papież Bonifacy IX przyznaje Katarzynie, wdowie po Paszku z Kleparza, łaskę, by w obliczu śmierci wybrany przez nią spowiednik mógł jeden raz udzielić jej mocą władzy apostolskiej pełnego odpuszczenia grzechów, pod określonymi warunkami."</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
           <t>Q400</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr"/>
@@ -4446,30 +4381,54 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"AAV, Reg. Lat., vol. 34, f. 172v"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Q401</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>"172v"</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
           <t>Q400</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr"/>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
@@ -4485,12 +4444,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>+1393-12-09T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -4524,44 +4483,28 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Q30</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>P30</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I99" t="inlineStr">
-        <is>
           <t>Q400</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr"/>
@@ -4574,27 +4517,27 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>P56</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>"BP 3, nr 349 (false sub data 9 XI 1393)"</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q385</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -4621,17 +4564,17 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>P33</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -4644,16 +4587,8 @@
           <t>Q400</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>Q400</t>
-        </is>
-      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
@@ -4668,17 +4603,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>P23</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
           <t>Q404</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>P2</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Q372</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4712,12 +4647,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -4746,17 +4681,17 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P38</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Q404</t>
+          <t>"Katherine, relicte quondam Peszkonis dicti de Florencia laici, vidue Cracouiensis diocesis"</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -4790,28 +4725,44 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Q413</t>
+          <t>"N(icolaus). XIIII. de Ben(even)to."</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P31</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
           <t>Q400</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
@@ -4824,17 +4775,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Q400</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P56</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4863,17 +4814,17 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P33</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Q402</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4883,7 +4834,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F107" t="inlineStr"/>
@@ -4902,17 +4853,17 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>P24</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Q392</t>
+          <t>Q372</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4922,7 +4873,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F108" t="inlineStr"/>
@@ -4941,17 +4892,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Q387</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4961,7 +4912,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F109" t="inlineStr"/>
@@ -4980,17 +4931,17 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>P11</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
+          <t>Q404</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -5000,7 +4951,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F110" t="inlineStr"/>
@@ -5019,69 +4970,37 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>"AAV, Reg. Lat., vol. 6, f. 257r-258v (or. f. CCLVII-CCLVIII)"</t>
+          <t>Q413</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>P20</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Q388</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>P14</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>Q382</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>"257r-258v"</t>
-        </is>
-      </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>P16</t>
-        </is>
-      </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>"CCLVII-CCLVIII"</t>
-        </is>
-      </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>Q381</t>
-        </is>
-      </c>
+          <t>Q400</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
       <c r="N111" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
       <c r="P111" t="inlineStr"/>
@@ -5090,17 +5009,17 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>P12</t>
+          <t>P27</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>+1389-11-13T00:00:00Z/11/J</t>
+          <t>Q30</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -5110,7 +5029,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q400</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
@@ -5134,12 +5053,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>P13</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Q31</t>
+          <t>Q402</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -5173,34 +5092,26 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P24</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>"MPV 8, nr 31"</t>
+          <t>Q392</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Q385</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
           <t>Q381</t>
         </is>
       </c>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
@@ -5220,34 +5131,26 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P19</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>"BP 3, nr 111"</t>
+          <t>Q387</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
           <t>Q381</t>
         </is>
       </c>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
@@ -5267,34 +5170,26 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>P17</t>
+          <t>P11</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>"RG 2, nr 05985"</t>
+          <t>"Papież Bonifacy IX poleca kustoszowi gnieźnieńskiemu, by mocą władzy apostolskiej udzielił szlachetnemu Mikołajowi Pieniążkowi z Węchadłowa i Witowic ekspektatywy na kanonię łęczycką, pomimo że Mikołaj posiada już kanonię gnieźnieńską i archidiakonat łęczycki, a ponadto otrzymał niedawno papieskie ekspektatywy na prałaturę w kapitule łęczyckiej (pod warunkiem opuszczenia archidiakonatu w razie jej objęcia) oraz na kanonię krakowską, a dzisiaj otrzymał także papieską ekspektatywę na kanonię uniejowską."</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>P18</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Q386</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
           <t>Q381</t>
         </is>
       </c>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr"/>
@@ -5314,32 +5209,64 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>P22</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>"AAV, Reg. Lat., vol. 6, f. 257r-258v (or. f. CCLVII-CCLVIII)"</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P20</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
+          <t>Q388</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>P14</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Q382</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>"257r-258v"</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>P16</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>"CCLVII-CCLVIII"</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr"/>
-      <c r="G117" t="inlineStr"/>
-      <c r="H117" t="inlineStr"/>
-      <c r="I117" t="inlineStr"/>
-      <c r="J117" t="inlineStr"/>
-      <c r="K117" t="inlineStr"/>
-      <c r="L117" t="inlineStr"/>
-      <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr"/>
       <c r="O117" t="inlineStr"/>
       <c r="P117" t="inlineStr"/>
@@ -5353,12 +5280,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>P23</t>
+          <t>P12</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Q391</t>
+          <t>+1389-11-13T00:00:00Z/11/J</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -5392,12 +5319,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>P25</t>
+          <t>P13</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>Q31</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -5431,26 +5358,34 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>P52</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>"MPV 8, nr 31"</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
+          <t>Q385</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr"/>
-      <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr"/>
@@ -5470,26 +5405,34 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>"C(ancellaria)"</t>
+          <t>"BP 3, nr 111"</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>S51</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
+          <t>Q386</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr"/>
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
@@ -5509,44 +5452,36 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>P34</t>
+          <t>P17</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>"N(icolaus). XXIIII. de Ben(even)to."</t>
+          <t>"RG 2, nr 05985"</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>P31</t>
+          <t>P18</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Q30</t>
+          <t>Q386</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>P30</t>
+          <t>S51</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="I122" t="inlineStr">
-        <is>
           <t>Q381</t>
         </is>
       </c>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
@@ -5559,17 +5494,17 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>P53</t>
+          <t>P22</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Q142</t>
+          <t>Q10</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -5598,17 +5533,17 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Q142</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>P35</t>
+          <t>P23</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>Q391</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -5637,17 +5572,17 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>Q381</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P25</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Q139</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -5681,12 +5616,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P52</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Q10</t>
+          <t>Q394</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -5720,12 +5655,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Q393</t>
+          <t>"C(ancellaria)"</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -5759,28 +5694,44 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P34</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
+          <t>"N(icolaus). XXIIII. de Ben(even)to."</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>P31</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
           <t>Q30</t>
         </is>
       </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>S51</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr">
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>P30</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
         <is>
           <t>Q381</t>
         </is>
       </c>
-      <c r="F128" t="inlineStr"/>
-      <c r="G128" t="inlineStr"/>
-      <c r="H128" t="inlineStr"/>
-      <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr"/>
@@ -5793,17 +5744,17 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Q391</t>
+          <t>Q142</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -5832,17 +5783,17 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q142</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Q142</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -5871,17 +5822,17 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Q394</t>
+          <t>Q142</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -5910,17 +5861,17 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q142</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Q118</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -5949,12 +5900,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P53</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -5988,17 +5939,17 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q398</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P35</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Q149</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -6027,17 +5978,17 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Q381</t>
+          <t>Q393</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>P27</t>
+          <t>P54</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Q146</t>
+          <t>Q394</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -6063,6 +6014,669 @@
       <c r="P135" t="inlineStr"/>
       <c r="Q135" t="inlineStr"/>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Q394</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>P28</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr"/>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
+      <c r="K136" t="inlineStr"/>
+      <c r="L136" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" t="inlineStr"/>
+      <c r="Q136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>P54</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Q149</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr"/>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
+      <c r="K137" t="inlineStr"/>
+      <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" t="inlineStr"/>
+      <c r="Q137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Q149</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>P28</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
+      <c r="K138" t="inlineStr"/>
+      <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" t="inlineStr"/>
+      <c r="Q138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>P54</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Q146</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
+      <c r="K139" t="inlineStr"/>
+      <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr"/>
+      <c r="P139" t="inlineStr"/>
+      <c r="Q139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Q146</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>P28</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr"/>
+      <c r="K140" t="inlineStr"/>
+      <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" t="inlineStr"/>
+      <c r="O140" t="inlineStr"/>
+      <c r="P140" t="inlineStr"/>
+      <c r="Q140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Q391</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>P29</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Q416</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr"/>
+      <c r="K141" t="inlineStr"/>
+      <c r="L141" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
+      <c r="P141" t="inlineStr"/>
+      <c r="Q141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Q394</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Q139</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
+      <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
+      <c r="N142" t="inlineStr"/>
+      <c r="O142" t="inlineStr"/>
+      <c r="P142" t="inlineStr"/>
+      <c r="Q142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Q10</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
+      <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
+      <c r="P143" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Q393</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" t="inlineStr"/>
+      <c r="K144" t="inlineStr"/>
+      <c r="L144" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
+      <c r="P144" t="inlineStr"/>
+      <c r="Q144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Q30</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
+      <c r="K145" t="inlineStr"/>
+      <c r="L145" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Q391</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
+      <c r="K146" t="inlineStr"/>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+      <c r="Q146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Q142</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" t="inlineStr"/>
+      <c r="K147" t="inlineStr"/>
+      <c r="L147" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Q394</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
+      <c r="L148" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
+      <c r="P148" t="inlineStr"/>
+      <c r="Q148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Q118</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
+      <c r="L149" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" t="inlineStr"/>
+      <c r="Q149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Q398</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
+      <c r="K150" t="inlineStr"/>
+      <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" t="inlineStr"/>
+      <c r="Q150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Q149</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" t="inlineStr"/>
+      <c r="Q151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>P27</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Q146</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Q381</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
+      <c r="L152" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr"/>
+      <c r="O152" t="inlineStr"/>
+      <c r="P152" t="inlineStr"/>
+      <c r="Q152" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Skrypt - poprawione miejsce wystawienia
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -653,7 +653,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>va-Q67</t>
+          <t>Q67</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1520,7 +1520,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>va-Q67</t>
+          <t>Q67</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>va-Q67</t>
+          <t>Q67</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>va-Q67</t>
+          <t>Q67</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>va-Q67</t>
+          <t>Q67</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">

</xml_diff>